<commit_message>
feat: add data extractor
</commit_message>
<xml_diff>
--- a/pkg/parser/testdata/similar_transfers.xlsx
+++ b/pkg/parser/testdata/similar_transfers.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\iqpirat\sources\github\firefly-iii-privatbank-importer\pkg\parser\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renth\FOR_FUN_PROJECTS\firefly-iii-privatbank-importer\pkg\parser\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290590D3-B8CE-4C34-B4CA-41B04457B52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22E28EB-DBBA-47E4-81C5-C0FBE2499739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44910" yWindow="3900" windowWidth="34875" windowHeight="15345" xr2:uid="{E22DDD79-B59B-415F-BC70-9DC0290099ED}"/>
+    <workbookView xWindow="3675" yWindow="1095" windowWidth="25665" windowHeight="20505" xr2:uid="{E22DDD79-B59B-415F-BC70-9DC0290099ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>PLN</t>
   </si>
@@ -56,6 +56,42 @@
   <si>
     <t>Konto Osobiste
 22222222222222222222222222</t>
+  </si>
+  <si>
+    <t>Data transakcji</t>
+  </si>
+  <si>
+    <t>Data zaksięgowania</t>
+  </si>
+  <si>
+    <t>Data odrzucenia</t>
+  </si>
+  <si>
+    <t>Kwota</t>
+  </si>
+  <si>
+    <t>Waluta</t>
+  </si>
+  <si>
+    <t>Nadawca / odbiorca</t>
+  </si>
+  <si>
+    <t>Opis</t>
+  </si>
+  <si>
+    <t>Produkt</t>
+  </si>
+  <si>
+    <t>Typ transakcji</t>
+  </si>
+  <si>
+    <t>Kwota zlecenia</t>
+  </si>
+  <si>
+    <t>Waluta zlecenia</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -66,7 +102,7 @@
     <numFmt numFmtId="164" formatCode="#\ ##0.00"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,13 +117,26 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF009D6A"/>
+        <bgColor rgb="FF008080"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -103,7 +152,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -111,6 +160,9 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,21 +498,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864D744B-7182-43F5-B379-82C3AD3D72B5}">
-  <dimension ref="A2:L3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="48.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" customWidth="1"/>
-    <col min="6" max="6" width="36.42578125" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" customWidth="1"/>
+    <col min="1" max="1" width="48.59765625" customWidth="1"/>
+    <col min="2" max="2" width="43.86328125" customWidth="1"/>
+    <col min="6" max="6" width="36.3984375" customWidth="1"/>
+    <col min="8" max="8" width="43.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="4">
         <v>45352</v>
       </c>
@@ -496,7 +586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
         <v>45352</v>
       </c>

</xml_diff>

<commit_message>
Fix Paribas parser (#33)
* feat: add data extractor

* fix: tests

* feat: fix for credit repayment

* feat: add new logic for credit transactions

* feat: add additional check

* feat: fix tx with parsing errors

* feat: remove print logs
</commit_message>
<xml_diff>
--- a/pkg/parser/testdata/similar_transfers.xlsx
+++ b/pkg/parser/testdata/similar_transfers.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\iqpirat\sources\github\firefly-iii-privatbank-importer\pkg\parser\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renth\FOR_FUN_PROJECTS\firefly-iii-privatbank-importer\pkg\parser\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290590D3-B8CE-4C34-B4CA-41B04457B52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22E28EB-DBBA-47E4-81C5-C0FBE2499739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44910" yWindow="3900" windowWidth="34875" windowHeight="15345" xr2:uid="{E22DDD79-B59B-415F-BC70-9DC0290099ED}"/>
+    <workbookView xWindow="3675" yWindow="1095" windowWidth="25665" windowHeight="20505" xr2:uid="{E22DDD79-B59B-415F-BC70-9DC0290099ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>PLN</t>
   </si>
@@ -56,6 +56,42 @@
   <si>
     <t>Konto Osobiste
 22222222222222222222222222</t>
+  </si>
+  <si>
+    <t>Data transakcji</t>
+  </si>
+  <si>
+    <t>Data zaksięgowania</t>
+  </si>
+  <si>
+    <t>Data odrzucenia</t>
+  </si>
+  <si>
+    <t>Kwota</t>
+  </si>
+  <si>
+    <t>Waluta</t>
+  </si>
+  <si>
+    <t>Nadawca / odbiorca</t>
+  </si>
+  <si>
+    <t>Opis</t>
+  </si>
+  <si>
+    <t>Produkt</t>
+  </si>
+  <si>
+    <t>Typ transakcji</t>
+  </si>
+  <si>
+    <t>Kwota zlecenia</t>
+  </si>
+  <si>
+    <t>Waluta zlecenia</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -66,7 +102,7 @@
     <numFmt numFmtId="164" formatCode="#\ ##0.00"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,13 +117,26 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF009D6A"/>
+        <bgColor rgb="FF008080"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -103,7 +152,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -111,6 +160,9 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,21 +498,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864D744B-7182-43F5-B379-82C3AD3D72B5}">
-  <dimension ref="A2:L3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="48.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" customWidth="1"/>
-    <col min="6" max="6" width="36.42578125" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" customWidth="1"/>
+    <col min="1" max="1" width="48.59765625" customWidth="1"/>
+    <col min="2" max="2" width="43.86328125" customWidth="1"/>
+    <col min="6" max="6" width="36.3984375" customWidth="1"/>
+    <col min="8" max="8" width="43.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="4">
         <v>45352</v>
       </c>
@@ -496,7 +586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
         <v>45352</v>
       </c>

</xml_diff>